<commit_message>
translate the formula downwards
</commit_message>
<xml_diff>
--- a/samplecode/books/21/21.turnover_worker.xlsx
+++ b/samplecode/books/21/21.turnover_worker.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yokotam\Documents\GitHub\python_excel_zenbuiri\20_SampleCode\Chapter2\Section021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685B70F2-4245-4F6B-9B7D-A484933F00BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42490CC2-96A2-46DA-AD6F-369741E19D10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5310" yWindow="5730" windowWidth="19035" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7710" yWindow="9585" windowWidth="19035" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="4月" sheetId="1" r:id="rId1"/>
+    <sheet name="202004" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -32,48 +35,128 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
+    <t>名前</t>
+    <rPh sb="0" eb="2">
+      <t>ナマエ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>売価</t>
+    <rPh sb="0" eb="2">
+      <t>バイカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>新井太郎</t>
+    <rPh sb="0" eb="2">
+      <t>アライ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>タロウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>鈴木一</t>
+    <rPh sb="0" eb="2">
+      <t>スズキ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ハジメ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>田中さちえ</t>
+    <rPh sb="0" eb="2">
+      <t>タナカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>谷口誠</t>
+    <rPh sb="0" eb="2">
+      <t>タニグチ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>マコト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>川上恵</t>
+    <rPh sb="0" eb="2">
+      <t>カワカミ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>メグミ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>斉藤厚</t>
+    <rPh sb="0" eb="2">
+      <t>サイトウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>アツシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>水野翔太</t>
+    <rPh sb="0" eb="1">
+      <t>ミズ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ショウタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>森下弘樹</t>
+    <rPh sb="0" eb="2">
+      <t>モリシタ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ヒロキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>原価</t>
+    <rPh sb="0" eb="2">
+      <t>ゲンカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>売価合計</t>
+    <rPh sb="0" eb="2">
+      <t>バイカ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ゴウケイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>粗利合計</t>
-  </si>
-  <si>
-    <t>名前</t>
-  </si>
-  <si>
-    <t>新井太郎</t>
-  </si>
-  <si>
-    <t>鈴木一</t>
-  </si>
-  <si>
-    <t>田中さちえ</t>
-  </si>
-  <si>
-    <t>谷口誠</t>
-  </si>
-  <si>
-    <t>川上恵</t>
-  </si>
-  <si>
-    <t>斉藤厚</t>
-  </si>
-  <si>
-    <t>水野翔太</t>
-  </si>
-  <si>
-    <t>森下弘樹</t>
-  </si>
-  <si>
-    <t>原価</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>売価</t>
+    <rPh sb="0" eb="2">
+      <t>アラリ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ゴウケイ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>粗利</t>
+    <rPh sb="0" eb="2">
+      <t>アラリ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -147,9 +230,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -437,23 +521,21 @@
   <dimension ref="A2:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="11.625" customWidth="1"/>
-    <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="13.875" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="2" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4">
-      <c r="C2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -464,22 +546,22 @@
       <c r="D3" s="1"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="A5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="1">
         <v>774000</v>
@@ -487,11 +569,13 @@
       <c r="C6" s="1">
         <v>900000</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="2">
+        <v>126000</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1">
         <v>680000</v>
@@ -499,11 +583,13 @@
       <c r="C7" s="1">
         <v>765000</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="2">
+        <v>85000</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1">
         <v>728000</v>
@@ -511,11 +597,13 @@
       <c r="C8" s="1">
         <v>819000</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="2">
+        <v>91000</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1">
         <v>528000</v>
@@ -523,11 +611,13 @@
       <c r="C9" s="1">
         <v>660000</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="2">
+        <v>132000</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1">
         <v>550400</v>
@@ -535,11 +625,13 @@
       <c r="C10" s="1">
         <v>688000</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="2">
+        <v>137600</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1">
         <v>496000</v>
@@ -547,11 +639,13 @@
       <c r="C11" s="1">
         <v>620000</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="2">
+        <v>124000</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1">
         <v>534400</v>
@@ -559,11 +653,13 @@
       <c r="C12" s="1">
         <v>668000</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="2">
+        <v>133600</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="1">
         <v>547200</v>
@@ -571,11 +667,13 @@
       <c r="C13" s="1">
         <v>684000</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="2">
+        <v>136800</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="1">
         <v>534400</v>
@@ -583,11 +681,13 @@
       <c r="C14" s="1">
         <v>668000</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="2">
+        <v>133600</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" s="1">
         <v>547200</v>
@@ -595,7 +695,9 @@
       <c r="C15" s="1">
         <v>684000</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="2">
+        <v>136800</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>